<commit_message>
added java and egde exe, also modified acg workbook
</commit_message>
<xml_diff>
--- a/ACG_Common_Workbook.xlsx
+++ b/ACG_Common_Workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse Docs\Selenium Test Case\ACG_Life_Science_Cloud\NEW_L4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kalpita_Jenkins\L4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F99A2ED-D58F-4D51-95FB-FB371BE0BDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A05977-1E6D-4088-AF41-28C0899604E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="URL_Login_cred_Tenant" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Users" sheetId="5" r:id="rId5"/>
     <sheet name="Password_Complex" sheetId="6" r:id="rId6"/>
     <sheet name="partner" sheetId="7" r:id="rId7"/>
+    <sheet name="Product" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="231">
   <si>
     <t>URL</t>
   </si>
@@ -627,6 +628,111 @@
   </si>
   <si>
     <t>ACG3207@gmail.com</t>
+  </si>
+  <si>
+    <t>ProductIdentifier</t>
+  </si>
+  <si>
+    <t>ProductName</t>
+  </si>
+  <si>
+    <t>Product Description</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>GS1 Company Prefix</t>
+  </si>
+  <si>
+    <t>GLN</t>
+  </si>
+  <si>
+    <t>PackagingLevelIndicator</t>
+  </si>
+  <si>
+    <t>Generic Name</t>
+  </si>
+  <si>
+    <t>Min Temp</t>
+  </si>
+  <si>
+    <t>weight (gm)</t>
+  </si>
+  <si>
+    <t>Strength (mg)</t>
+  </si>
+  <si>
+    <t>Product1</t>
+  </si>
+  <si>
+    <t>Gemcitabine Injection 200mg/ 5.26mL</t>
+  </si>
+  <si>
+    <t>manufacturer1</t>
+  </si>
+  <si>
+    <t>testMed1</t>
+  </si>
+  <si>
+    <t>Product2</t>
+  </si>
+  <si>
+    <t>Gemcitabine Injection 200mg/ 5.27mL</t>
+  </si>
+  <si>
+    <t>manufacturer2</t>
+  </si>
+  <si>
+    <t>testMed2</t>
+  </si>
+  <si>
+    <t>Product3</t>
+  </si>
+  <si>
+    <t>Gemcitabine Injection 200mg/ 5.28mL</t>
+  </si>
+  <si>
+    <t>manufacturer3</t>
+  </si>
+  <si>
+    <t>testMed3</t>
+  </si>
+  <si>
+    <t>Product4</t>
+  </si>
+  <si>
+    <t>manufacturer4</t>
+  </si>
+  <si>
+    <t>testMed4</t>
+  </si>
+  <si>
+    <t>Product5</t>
+  </si>
+  <si>
+    <t>Gemcitabine Injection 200mg/ 5.29mL</t>
+  </si>
+  <si>
+    <t>manufacturer5</t>
+  </si>
+  <si>
+    <t>testMed5</t>
+  </si>
+  <si>
+    <t>890877002005</t>
+  </si>
+  <si>
+    <t>890877002006</t>
+  </si>
+  <si>
+    <t>890877002007</t>
+  </si>
+  <si>
+    <t>890877002008</t>
+  </si>
+  <si>
+    <t>890877002009</t>
   </si>
 </sst>
 </file>
@@ -1878,7 +1984,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -2533,12 +2639,21 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -2918,4 +3033,261 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DECABE2-820C-482A-8F9E-9586007BAFE9}">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.08984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G1" t="s">
+        <v>196</v>
+      </c>
+      <c r="H1" t="s">
+        <v>202</v>
+      </c>
+      <c r="I1" t="s">
+        <v>203</v>
+      </c>
+      <c r="J1" t="s">
+        <v>204</v>
+      </c>
+      <c r="K1" t="s">
+        <v>205</v>
+      </c>
+      <c r="L1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>515364</v>
+      </c>
+      <c r="B2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2">
+        <v>515362</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="G2">
+        <v>515362</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>210</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>515363</v>
+      </c>
+      <c r="B3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" t="s">
+        <v>212</v>
+      </c>
+      <c r="D3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E3">
+        <v>515363</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="G3">
+        <v>515363</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>214</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>515362</v>
+      </c>
+      <c r="B4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" t="s">
+        <v>216</v>
+      </c>
+      <c r="D4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E4">
+        <v>515364</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="G4">
+        <v>515364</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>218</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>515365</v>
+      </c>
+      <c r="B5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E5">
+        <v>515365</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>229</v>
+      </c>
+      <c r="G5">
+        <v>515365</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>221</v>
+      </c>
+      <c r="J5">
+        <v>8</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>515366</v>
+      </c>
+      <c r="B6" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E6">
+        <v>515366</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="G6">
+        <v>515366</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>225</v>
+      </c>
+      <c r="J6">
+        <v>9</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <v>4.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added product and location py file, deleted java files
</commit_message>
<xml_diff>
--- a/ACG_Common_Workbook.xlsx
+++ b/ACG_Common_Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kalpita_Jenkins\L4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0A05977-1E6D-4088-AF41-28C0899604E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5C1FEE-E61F-492C-8B5F-9BC24497F3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="URL_Login_cred_Tenant" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="230">
   <si>
     <t>URL</t>
   </si>
@@ -663,18 +663,6 @@
     <t>Strength (mg)</t>
   </si>
   <si>
-    <t>Product1</t>
-  </si>
-  <si>
-    <t>Gemcitabine Injection 200mg/ 5.26mL</t>
-  </si>
-  <si>
-    <t>manufacturer1</t>
-  </si>
-  <si>
-    <t>testMed1</t>
-  </si>
-  <si>
     <t>Product2</t>
   </si>
   <si>
@@ -720,19 +708,28 @@
     <t>testMed5</t>
   </si>
   <si>
-    <t>890877002005</t>
-  </si>
-  <si>
-    <t>890877002006</t>
-  </si>
-  <si>
-    <t>890877002007</t>
-  </si>
-  <si>
-    <t>890877002008</t>
-  </si>
-  <si>
-    <t>890877002009</t>
+    <t>8908770020062</t>
+  </si>
+  <si>
+    <t>8908770020073</t>
+  </si>
+  <si>
+    <t>8908770020084</t>
+  </si>
+  <si>
+    <t>8908770020095</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>Business entity</t>
+  </si>
+  <si>
+    <t>Location_Type</t>
+  </si>
+  <si>
+    <t>Packaging Site</t>
   </si>
 </sst>
 </file>
@@ -2636,10 +2633,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2654,358 +2651,460 @@
     <col min="8" max="8" width="18.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.81640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="K1" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>364850</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>7647</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="1">
         <v>9579532456</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="K2" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>364851</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>7647</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>9579532456</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="K3" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>364852</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="1">
         <v>7647</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="1">
         <v>9579532456</v>
       </c>
-      <c r="J4" s="16" t="s">
+      <c r="J4" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="K4" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>364853</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>7647</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="1">
         <v>9579532456</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="K5" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>364854</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>7647</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="1">
         <v>9579532456</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="J6" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="K6" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>364855</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>7647</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="1">
         <v>9579532456</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="J7" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="K7" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>364856</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>7647</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="1">
         <v>9579532456</v>
       </c>
-      <c r="J8" s="16" t="s">
+      <c r="J8" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="K8" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>364857</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>7647</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H9" s="16" t="s">
+      <c r="H9" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <v>9579532456</v>
       </c>
-      <c r="J9" s="16" t="s">
+      <c r="J9" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="K9" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>364858</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="1">
         <v>7647</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="1">
         <v>9579532456</v>
       </c>
-      <c r="J10" s="16" t="s">
+      <c r="J10" s="4" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="K10" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>364859</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>7647</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="1">
         <v>9579532456</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="4" t="s">
         <v>161</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -3037,10 +3136,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DECABE2-820C-482A-8F9E-9586007BAFE9}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3050,7 +3149,7 @@
     <col min="3" max="3" width="32.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.7265625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.54296875" bestFit="1" customWidth="1"/>
@@ -3060,230 +3159,192 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2">
+      <c r="A2" s="1">
+        <v>515363</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="E2" s="1">
+        <v>515363</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="G2" s="1">
+        <v>515363</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="J2" s="1">
+        <v>6</v>
+      </c>
+      <c r="K2" s="1">
+        <v>1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>515362</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E3" s="1">
         <v>515364</v>
       </c>
-      <c r="B2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D2" t="s">
-        <v>209</v>
-      </c>
-      <c r="E2">
-        <v>515362</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>226</v>
-      </c>
-      <c r="G2">
-        <v>515362</v>
-      </c>
-      <c r="H2">
+      <c r="F3" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G3" s="1">
+        <v>515364</v>
+      </c>
+      <c r="H3" s="1">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
-        <v>210</v>
-      </c>
-      <c r="J2">
-        <v>5</v>
-      </c>
-      <c r="K2">
+      <c r="I3" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="J3" s="1">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1">
         <v>1</v>
       </c>
-      <c r="L2">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>515363</v>
-      </c>
-      <c r="B3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="L3" s="1">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>515365</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="D3" t="s">
-        <v>213</v>
-      </c>
-      <c r="E3">
-        <v>515363</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G3">
-        <v>515363</v>
-      </c>
-      <c r="H3">
+      <c r="D4" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E4" s="1">
+        <v>515365</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="G4" s="1">
+        <v>515365</v>
+      </c>
+      <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="I3" t="s">
-        <v>214</v>
-      </c>
-      <c r="J3">
-        <v>6</v>
-      </c>
-      <c r="K3">
+      <c r="I4" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="J4" s="1">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1">
         <v>1</v>
       </c>
-      <c r="L3">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>515362</v>
-      </c>
-      <c r="B4" t="s">
-        <v>215</v>
-      </c>
-      <c r="C4" t="s">
-        <v>216</v>
-      </c>
-      <c r="D4" t="s">
-        <v>217</v>
-      </c>
-      <c r="E4">
-        <v>515364</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>228</v>
-      </c>
-      <c r="G4">
-        <v>515364</v>
-      </c>
-      <c r="H4">
+      <c r="L4" s="1">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>515366</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="E5" s="1">
+        <v>515366</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="G5" s="1">
+        <v>515366</v>
+      </c>
+      <c r="H5" s="1">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
-        <v>218</v>
-      </c>
-      <c r="J4">
-        <v>7</v>
-      </c>
-      <c r="K4">
+      <c r="I5" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="J5" s="1">
+        <v>9</v>
+      </c>
+      <c r="K5" s="1">
         <v>1</v>
       </c>
-      <c r="L4">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>515365</v>
-      </c>
-      <c r="B5" t="s">
-        <v>219</v>
-      </c>
-      <c r="C5" t="s">
-        <v>216</v>
-      </c>
-      <c r="D5" t="s">
-        <v>220</v>
-      </c>
-      <c r="E5">
-        <v>515365</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>229</v>
-      </c>
-      <c r="G5">
-        <v>515365</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>221</v>
-      </c>
-      <c r="J5">
-        <v>8</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>515366</v>
-      </c>
-      <c r="B6" t="s">
-        <v>222</v>
-      </c>
-      <c r="C6" t="s">
-        <v>223</v>
-      </c>
-      <c r="D6" t="s">
-        <v>224</v>
-      </c>
-      <c r="E6">
-        <v>515366</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>230</v>
-      </c>
-      <c r="G6">
-        <v>515366</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>225</v>
-      </c>
-      <c r="J6">
-        <v>9</v>
-      </c>
-      <c r="K6">
-        <v>1</v>
-      </c>
-      <c r="L6">
+      <c r="L5" s="1">
         <v>4.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modifed excel path and cell values
</commit_message>
<xml_diff>
--- a/ACG_Common_Workbook.xlsx
+++ b/ACG_Common_Workbook.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kalpita_Jenkins\L4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5C1FEE-E61F-492C-8B5F-9BC24497F3FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C686F1F9-BE54-42CE-B9A3-E749F47F542B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="219">
   <si>
     <t>URL</t>
   </si>
@@ -507,9 +507,6 @@
     <t>website</t>
   </si>
   <si>
-    <t>location1</t>
-  </si>
-  <si>
     <t>NJ</t>
   </si>
   <si>
@@ -528,60 +525,15 @@
     <t>www.demoo.com</t>
   </si>
   <si>
-    <t>location2</t>
-  </si>
-  <si>
     <t>136 Ludlow Ave</t>
   </si>
   <si>
-    <t>location3</t>
-  </si>
-  <si>
     <t>137 Ludlow Ave</t>
   </si>
   <si>
-    <t>location4</t>
-  </si>
-  <si>
     <t>138 Ludlow Ave</t>
   </si>
   <si>
-    <t>location5</t>
-  </si>
-  <si>
-    <t>139 Ludlow Ave</t>
-  </si>
-  <si>
-    <t>location6</t>
-  </si>
-  <si>
-    <t>140 Ludlow Ave</t>
-  </si>
-  <si>
-    <t>location7</t>
-  </si>
-  <si>
-    <t>141 Ludlow Ave</t>
-  </si>
-  <si>
-    <t>location8</t>
-  </si>
-  <si>
-    <t>142 Ludlow Ave</t>
-  </si>
-  <si>
-    <t>location9</t>
-  </si>
-  <si>
-    <t>143 Ludlow Ave</t>
-  </si>
-  <si>
-    <t>location10</t>
-  </si>
-  <si>
-    <t>144 Ludlow Ave</t>
-  </si>
-  <si>
     <t>ACG3200</t>
   </si>
   <si>
@@ -663,9 +615,6 @@
     <t>Strength (mg)</t>
   </si>
   <si>
-    <t>Product2</t>
-  </si>
-  <si>
     <t>Gemcitabine Injection 200mg/ 5.27mL</t>
   </si>
   <si>
@@ -675,9 +624,6 @@
     <t>testMed2</t>
   </si>
   <si>
-    <t>Product3</t>
-  </si>
-  <si>
     <t>Gemcitabine Injection 200mg/ 5.28mL</t>
   </si>
   <si>
@@ -687,18 +633,12 @@
     <t>testMed3</t>
   </si>
   <si>
-    <t>Product4</t>
-  </si>
-  <si>
     <t>manufacturer4</t>
   </si>
   <si>
     <t>testMed4</t>
   </si>
   <si>
-    <t>Product5</t>
-  </si>
-  <si>
     <t>Gemcitabine Injection 200mg/ 5.29mL</t>
   </si>
   <si>
@@ -708,18 +648,9 @@
     <t>testMed5</t>
   </si>
   <si>
-    <t>8908770020062</t>
-  </si>
-  <si>
-    <t>8908770020073</t>
-  </si>
-  <si>
     <t>8908770020084</t>
   </si>
   <si>
-    <t>8908770020095</t>
-  </si>
-  <si>
     <t>Entity</t>
   </si>
   <si>
@@ -730,6 +661,42 @@
   </si>
   <si>
     <t>Packaging Site</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>Product10</t>
+  </si>
+  <si>
+    <t>Product11</t>
+  </si>
+  <si>
+    <t>Product12</t>
+  </si>
+  <si>
+    <t>Product13</t>
+  </si>
+  <si>
+    <t>8908770020072</t>
+  </si>
+  <si>
+    <t>8908770020083</t>
+  </si>
+  <si>
+    <t>8908770020074</t>
+  </si>
+  <si>
+    <t>location13</t>
+  </si>
+  <si>
+    <t>location23</t>
+  </si>
+  <si>
+    <t>location32</t>
+  </si>
+  <si>
+    <t>location43</t>
   </si>
 </sst>
 </file>
@@ -2042,10 +2009,10 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="C2" s="3">
         <v>1234565450</v>
@@ -2075,7 +2042,7 @@
         <v>65</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>97</v>
@@ -2087,10 +2054,10 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="C3" s="3">
         <v>1234565451</v>
@@ -2120,7 +2087,7 @@
         <v>65</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>97</v>
@@ -2132,10 +2099,10 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="C4" s="3">
         <v>1234565452</v>
@@ -2165,7 +2132,7 @@
         <v>65</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="Q4" s="2" t="s">
         <v>97</v>
@@ -2177,10 +2144,10 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="C5" s="3">
         <v>1234565453</v>
@@ -2204,7 +2171,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="P5" s="1" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="Q5" s="2" t="s">
         <v>97</v>
@@ -2216,10 +2183,10 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="C6" s="3">
         <v>1234565454</v>
@@ -2243,7 +2210,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="P6" s="1" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="Q6" s="2" t="s">
         <v>97</v>
@@ -2255,10 +2222,10 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="C7" s="3">
         <v>1234565455</v>
@@ -2282,7 +2249,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="P7" s="1" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>97</v>
@@ -2294,10 +2261,10 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="C8" s="3">
         <v>1234565456</v>
@@ -2321,7 +2288,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="P8" s="1" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="Q8" s="2" t="s">
         <v>97</v>
@@ -2333,10 +2300,10 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="C9" s="3">
         <v>1234565457</v>
@@ -2360,7 +2327,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="P9" s="1" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>97</v>
@@ -2633,10 +2600,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2688,423 +2655,177 @@
         <v>154</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="1">
+        <v>364445</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B2" s="1">
-        <v>364850</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>158</v>
       </c>
       <c r="F2" s="1">
         <v>7647</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="I2" s="1">
         <v>9579532456</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>94</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>162</v>
+        <v>216</v>
       </c>
       <c r="B3" s="1">
-        <v>364851</v>
+        <v>364446</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F3" s="1">
         <v>7647</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="I3" s="1">
         <v>9579532456</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>94</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>164</v>
+        <v>217</v>
       </c>
       <c r="B4" s="1">
-        <v>364852</v>
+        <v>364447</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="F4" s="1">
         <v>7647</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="I4" s="1">
         <v>9579532456</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>94</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>166</v>
+        <v>218</v>
       </c>
       <c r="B5" s="1">
-        <v>364853</v>
+        <v>364448</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>157</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F5" s="1">
         <v>7647</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>159</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="I5" s="1">
         <v>9579532456</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="L5" s="1" t="s">
         <v>94</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B6" s="1">
-        <v>364854</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="F6" s="1">
-        <v>7647</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="I6" s="1">
-        <v>9579532456</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B7" s="1">
-        <v>364855</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="F7" s="1">
-        <v>7647</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="I7" s="1">
-        <v>9579532456</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B8" s="1">
-        <v>364856</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F8" s="1">
-        <v>7647</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="I8" s="1">
-        <v>9579532456</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B9" s="1">
-        <v>364857</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="F9" s="1">
-        <v>7647</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="I9" s="1">
-        <v>9579532456</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B10" s="1">
-        <v>364858</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F10" s="1">
-        <v>7647</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="I10" s="1">
-        <v>9579532456</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M10" s="1" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B11" s="1">
-        <v>364859</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="F11" s="1">
-        <v>7647</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="I11" s="1">
-        <v>9579532456</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -3117,18 +2838,6 @@
     <hyperlink ref="J4" r:id="rId6" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
     <hyperlink ref="H5" r:id="rId7" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
     <hyperlink ref="J5" r:id="rId8" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
-    <hyperlink ref="H6" r:id="rId9" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
-    <hyperlink ref="J6" r:id="rId10" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
-    <hyperlink ref="H7" r:id="rId11" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
-    <hyperlink ref="J7" r:id="rId12" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
-    <hyperlink ref="H8" r:id="rId13" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
-    <hyperlink ref="J8" r:id="rId14" xr:uid="{00000000-0004-0000-0600-00000D000000}"/>
-    <hyperlink ref="H9" r:id="rId15" xr:uid="{00000000-0004-0000-0600-00000E000000}"/>
-    <hyperlink ref="J9" r:id="rId16" xr:uid="{00000000-0004-0000-0600-00000F000000}"/>
-    <hyperlink ref="H10" r:id="rId17" xr:uid="{00000000-0004-0000-0600-000010000000}"/>
-    <hyperlink ref="J10" r:id="rId18" xr:uid="{00000000-0004-0000-0600-000011000000}"/>
-    <hyperlink ref="H11" r:id="rId19" xr:uid="{00000000-0004-0000-0600-000012000000}"/>
-    <hyperlink ref="J11" r:id="rId20" xr:uid="{00000000-0004-0000-0600-000013000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3136,10 +2845,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DECABE2-820C-482A-8F9E-9586007BAFE9}">
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3160,60 +2869,60 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>515363</v>
+        <v>515373</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>208</v>
+        <v>191</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>209</v>
+        <v>192</v>
       </c>
       <c r="E2" s="1">
-        <v>515363</v>
+        <v>515373</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="G2" s="1">
         <v>515363</v>
@@ -3222,7 +2931,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>210</v>
+        <v>193</v>
       </c>
       <c r="J2" s="1">
         <v>6</v>
@@ -3236,22 +2945,22 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>515362</v>
+        <v>515374</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E3" s="1">
+        <v>515374</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="E3" s="1">
-        <v>515364</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>223</v>
       </c>
       <c r="G3" s="1">
         <v>515364</v>
@@ -3260,7 +2969,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="J3" s="1">
         <v>7</v>
@@ -3274,22 +2983,22 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>515365</v>
+        <v>515375</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>216</v>
+        <v>197</v>
       </c>
       <c r="E4" s="1">
-        <v>515365</v>
+        <v>515375</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="G4" s="1">
         <v>515365</v>
@@ -3298,7 +3007,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>217</v>
+        <v>198</v>
       </c>
       <c r="J4" s="1">
         <v>8</v>
@@ -3312,22 +3021,22 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>515366</v>
+        <v>515376</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="E5" s="1">
-        <v>515366</v>
+        <v>515376</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="G5" s="1">
         <v>515366</v>
@@ -3336,7 +3045,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="J5" s="1">
         <v>9</v>
@@ -3348,7 +3057,13 @@
         <v>4.5</v>
       </c>
     </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="E10" t="s">
+        <v>207</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modifed excel path and cell values for product
</commit_message>
<xml_diff>
--- a/ACG_Common_Workbook.xlsx
+++ b/ACG_Common_Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kalpita_Jenkins\L4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C686F1F9-BE54-42CE-B9A3-E749F47F542B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9D3852-0639-445B-BFE7-E2139CA4731A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="URL_Login_cred_Tenant" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="218">
   <si>
     <t>URL</t>
   </si>
@@ -663,21 +663,6 @@
     <t>Packaging Site</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
-    <t>Product10</t>
-  </si>
-  <si>
-    <t>Product11</t>
-  </si>
-  <si>
-    <t>Product12</t>
-  </si>
-  <si>
-    <t>Product13</t>
-  </si>
-  <si>
     <t>8908770020072</t>
   </si>
   <si>
@@ -697,6 +682,18 @@
   </si>
   <si>
     <t>location43</t>
+  </si>
+  <si>
+    <t>Product14</t>
+  </si>
+  <si>
+    <t>Product15</t>
+  </si>
+  <si>
+    <t>Product16</t>
+  </si>
+  <si>
+    <t>Product17</t>
   </si>
 </sst>
 </file>
@@ -2602,7 +2599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2666,7 +2663,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="B2" s="1">
         <v>364445</v>
@@ -2707,7 +2704,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="B3" s="1">
         <v>364446</v>
@@ -2748,7 +2745,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B4" s="1">
         <v>364447</v>
@@ -2789,7 +2786,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B5" s="1">
         <v>364448</v>
@@ -2845,10 +2842,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DECABE2-820C-482A-8F9E-9586007BAFE9}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2907,10 +2904,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>515373</v>
+        <v>515381</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>191</v>
@@ -2919,13 +2916,13 @@
         <v>192</v>
       </c>
       <c r="E2" s="1">
-        <v>515373</v>
+        <v>515381</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="G2" s="1">
-        <v>515363</v>
+        <v>515381</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
@@ -2945,10 +2942,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>515374</v>
+        <v>515382</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>194</v>
@@ -2957,13 +2954,13 @@
         <v>195</v>
       </c>
       <c r="E3" s="1">
-        <v>515374</v>
+        <v>515382</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="G3" s="1">
-        <v>515364</v>
+        <v>515382</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
@@ -2983,10 +2980,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>515375</v>
+        <v>515383</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>194</v>
@@ -2995,13 +2992,13 @@
         <v>197</v>
       </c>
       <c r="E4" s="1">
-        <v>515375</v>
+        <v>515383</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G4" s="1">
-        <v>515365</v>
+        <v>515383</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
@@ -3021,10 +3018,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>515376</v>
+        <v>515384</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>199</v>
@@ -3033,13 +3030,13 @@
         <v>200</v>
       </c>
       <c r="E5" s="1">
-        <v>515376</v>
+        <v>515384</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>202</v>
       </c>
       <c r="G5" s="1">
-        <v>515366</v>
+        <v>515384</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
@@ -3055,11 +3052,6 @@
       </c>
       <c r="L5" s="1">
         <v>4.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="E10" t="s">
-        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change the values for product, location, user, role
</commit_message>
<xml_diff>
--- a/ACG_Common_Workbook.xlsx
+++ b/ACG_Common_Workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kalpita_Jenkins\L4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9D3852-0639-445B-BFE7-E2139CA4731A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942D3638-67A2-4D83-B4DD-1F33D0B50A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="URL_Login_cred_Tenant" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="213">
   <si>
     <t>URL</t>
   </si>
@@ -267,9 +267,6 @@
     <t>To create a role all rights</t>
   </si>
   <si>
-    <t>Admin_new3</t>
-  </si>
-  <si>
     <t>Related to admin</t>
   </si>
   <si>
@@ -279,9 +276,6 @@
     <t>To create a role with create rights</t>
   </si>
   <si>
-    <t>Creator_new</t>
-  </si>
-  <si>
     <t>Related to creator</t>
   </si>
   <si>
@@ -315,12 +309,6 @@
     <t>Rolen</t>
   </si>
   <si>
-    <t>ACG2200</t>
-  </si>
-  <si>
-    <t>ACG2200@gmail.com</t>
-  </si>
-  <si>
     <t>Supervisor</t>
   </si>
   <si>
@@ -336,12 +324,6 @@
     <t>@gmail.com</t>
   </si>
   <si>
-    <t>ACG2201</t>
-  </si>
-  <si>
-    <t>ACG2201@gmail.com</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
@@ -357,9 +339,6 @@
     <t>To create a user with same emailid which is already used</t>
   </si>
   <si>
-    <t>User not created</t>
-  </si>
-  <si>
     <t>Please select an appropriate role.</t>
   </si>
   <si>
@@ -534,54 +513,6 @@
     <t>138 Ludlow Ave</t>
   </si>
   <si>
-    <t>ACG3200</t>
-  </si>
-  <si>
-    <t>ACG3201</t>
-  </si>
-  <si>
-    <t>ACG3202</t>
-  </si>
-  <si>
-    <t>ACG3203</t>
-  </si>
-  <si>
-    <t>ACG3204</t>
-  </si>
-  <si>
-    <t>ACG3205</t>
-  </si>
-  <si>
-    <t>ACG3206</t>
-  </si>
-  <si>
-    <t>ACG3207</t>
-  </si>
-  <si>
-    <t>ACG3200@gmail.com</t>
-  </si>
-  <si>
-    <t>ACG3201@gmail.com</t>
-  </si>
-  <si>
-    <t>ACG3202@gmail.com</t>
-  </si>
-  <si>
-    <t>ACG3203@gmail.com</t>
-  </si>
-  <si>
-    <t>ACG3204@gmail.com</t>
-  </si>
-  <si>
-    <t>ACG3205@gmail.com</t>
-  </si>
-  <si>
-    <t>ACG3206@gmail.com</t>
-  </si>
-  <si>
-    <t>ACG3207@gmail.com</t>
-  </si>
-  <si>
     <t>ProductIdentifier</t>
   </si>
   <si>
@@ -672,28 +603,82 @@
     <t>8908770020074</t>
   </si>
   <si>
-    <t>location13</t>
-  </si>
-  <si>
-    <t>location23</t>
-  </si>
-  <si>
-    <t>location32</t>
-  </si>
-  <si>
-    <t>location43</t>
-  </si>
-  <si>
-    <t>Product14</t>
-  </si>
-  <si>
-    <t>Product15</t>
-  </si>
-  <si>
-    <t>Product16</t>
-  </si>
-  <si>
-    <t>Product17</t>
+    <t>location15</t>
+  </si>
+  <si>
+    <t>location25</t>
+  </si>
+  <si>
+    <t>location35</t>
+  </si>
+  <si>
+    <t>location45</t>
+  </si>
+  <si>
+    <t>Product20</t>
+  </si>
+  <si>
+    <t>Product21</t>
+  </si>
+  <si>
+    <t>Product22</t>
+  </si>
+  <si>
+    <t>Product23</t>
+  </si>
+  <si>
+    <t>ACG3300</t>
+  </si>
+  <si>
+    <t>ACG3301</t>
+  </si>
+  <si>
+    <t>ACG3302</t>
+  </si>
+  <si>
+    <t>ACG3303</t>
+  </si>
+  <si>
+    <t>ACG3304</t>
+  </si>
+  <si>
+    <t>ACG3305</t>
+  </si>
+  <si>
+    <t>ACG3306</t>
+  </si>
+  <si>
+    <t>ACG3307</t>
+  </si>
+  <si>
+    <t>ACG3300@gmail.com</t>
+  </si>
+  <si>
+    <t>ACG3301@gmail.com</t>
+  </si>
+  <si>
+    <t>ACG3302@gmail.com</t>
+  </si>
+  <si>
+    <t>ACG3303@gmail.com</t>
+  </si>
+  <si>
+    <t>ACG3304@gmail.com</t>
+  </si>
+  <si>
+    <t>ACG3305@gmail.com</t>
+  </si>
+  <si>
+    <t>ACG3306@gmail.com</t>
+  </si>
+  <si>
+    <t>ACG3307@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin22</t>
+  </si>
+  <si>
+    <t>Creator22</t>
   </si>
 </sst>
 </file>
@@ -1764,8 +1749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1774,6 +1759,7 @@
     <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.35">
@@ -1895,46 +1881,34 @@
         <v>74</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1946,7 +1920,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H2" sqref="H2:K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1958,7 +1932,7 @@
     <col min="5" max="5" width="13.36328125" style="14" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="32.26953125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="54.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" customWidth="1"/>
+    <col min="8" max="8" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.7265625" customWidth="1" collapsed="1"/>
     <col min="10" max="15" width="8.7265625" customWidth="1"/>
     <col min="16" max="16" width="9.36328125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1971,34 +1945,34 @@
   <sheetData>
     <row r="1" spans="1:18" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>85</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>87</v>
       </c>
       <c r="G1" s="6" t="s">
         <v>55</v>
       </c>
       <c r="H1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>88</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>58</v>
@@ -2006,332 +1980,298 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>164</v>
+        <v>195</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>172</v>
+        <v>203</v>
       </c>
       <c r="C2" s="3">
         <v>1234565450</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="P2" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="R2" t="str">
         <f t="shared" ref="R2:R9" si="0">_xlfn.CONCAT(P2,Q2)</f>
-        <v>ACG3200@gmail.com</v>
+        <v>ACG3300@gmail.com</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
       <c r="C3" s="3">
         <v>1234565451</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>65</v>
-      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="R3" t="str">
         <f t="shared" si="0"/>
-        <v>ACG3201@gmail.com</v>
+        <v>ACG3301@gmail.com</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>166</v>
+        <v>197</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>174</v>
+        <v>205</v>
       </c>
       <c r="C4" s="3">
         <v>1234565452</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="P4" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="R4" t="str">
         <f t="shared" si="0"/>
-        <v>ACG3202@gmail.com</v>
+        <v>ACG3302@gmail.com</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>167</v>
+        <v>198</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>175</v>
+        <v>206</v>
       </c>
       <c r="C5" s="3">
         <v>1234565453</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>105</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="P5" s="1" t="s">
-        <v>167</v>
+        <v>198</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="R5" t="str">
         <f t="shared" si="0"/>
-        <v>ACG3203@gmail.com</v>
+        <v>ACG3303@gmail.com</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>168</v>
+        <v>199</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>176</v>
+        <v>207</v>
       </c>
       <c r="C6" s="3">
         <v>1234565454</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="P6" s="1" t="s">
-        <v>168</v>
+        <v>199</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="R6" t="str">
         <f t="shared" si="0"/>
-        <v>ACG3204@gmail.com</v>
+        <v>ACG3304@gmail.com</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>169</v>
+        <v>200</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
       <c r="C7" s="3">
         <v>1234565455</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>105</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="P7" s="1" t="s">
-        <v>169</v>
+        <v>200</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="R7" t="str">
         <f t="shared" si="0"/>
-        <v>ACG3205@gmail.com</v>
+        <v>ACG3305@gmail.com</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="C8" s="3">
         <v>1234565456</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>105</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="P8" s="1" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="R8" t="str">
         <f t="shared" si="0"/>
-        <v>ACG3206@gmail.com</v>
+        <v>ACG3306@gmail.com</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>179</v>
+        <v>210</v>
       </c>
       <c r="C9" s="3">
         <v>1234565457</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>105</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="P9" s="1" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="R9" t="str">
         <f t="shared" si="0"/>
-        <v>ACG3207@gmail.com</v>
+        <v>ACG3307@gmail.com</v>
       </c>
     </row>
   </sheetData>
@@ -2381,96 +2321,96 @@
   <sheetData>
     <row r="1" spans="1:5" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -2479,100 +2419,100 @@
         <v>6</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="9" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="9" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="9" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="9" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2600,7 +2540,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B2" sqref="B2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2622,207 +2562,207 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>204</v>
+        <v>181</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="B2" s="1">
-        <v>364445</v>
+        <v>364450</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F2" s="1">
         <v>7647</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="I2" s="1">
         <v>9579532456</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="B3" s="1">
-        <v>364446</v>
+        <v>364451</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="F3" s="1">
         <v>7647</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="I3" s="1">
         <v>9579532456</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>212</v>
+        <v>189</v>
       </c>
       <c r="B4" s="1">
-        <v>364447</v>
+        <v>364452</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="F4" s="1">
         <v>7647</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="I4" s="1">
         <v>9579532456</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>213</v>
+        <v>190</v>
       </c>
       <c r="B5" s="1">
-        <v>364448</v>
+        <v>364453</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="F5" s="1">
         <v>7647</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="I5" s="1">
         <v>9579532456</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2844,7 +2784,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DECABE2-820C-482A-8F9E-9586007BAFE9}">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2:G5"/>
     </sheetView>
   </sheetViews>
@@ -2866,69 +2806,69 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>181</v>
+        <v>158</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>182</v>
+        <v>159</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>183</v>
+        <v>160</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>184</v>
+        <v>161</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>185</v>
+        <v>162</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>180</v>
+        <v>157</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>186</v>
+        <v>163</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>187</v>
+        <v>164</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>189</v>
+        <v>166</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>515381</v>
+        <v>515391</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>214</v>
+        <v>191</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>192</v>
+        <v>169</v>
       </c>
       <c r="E2" s="1">
-        <v>515381</v>
+        <v>515391</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>207</v>
+        <v>184</v>
       </c>
       <c r="G2" s="1">
-        <v>515381</v>
+        <v>515391</v>
       </c>
       <c r="H2" s="1">
         <v>1</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>193</v>
+        <v>170</v>
       </c>
       <c r="J2" s="1">
         <v>6</v>
@@ -2942,31 +2882,31 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
-        <v>515382</v>
+        <v>515392</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
+        <v>192</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>195</v>
+        <v>172</v>
       </c>
       <c r="E3" s="1">
-        <v>515382</v>
+        <v>515392</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="G3" s="1">
-        <v>515382</v>
+        <v>515392</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>196</v>
+        <v>173</v>
       </c>
       <c r="J3" s="1">
         <v>7</v>
@@ -2980,31 +2920,31 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>515383</v>
+        <v>515393</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>194</v>
+        <v>171</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>197</v>
+        <v>174</v>
       </c>
       <c r="E4" s="1">
-        <v>515383</v>
+        <v>515393</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>209</v>
+        <v>186</v>
       </c>
       <c r="G4" s="1">
-        <v>515383</v>
+        <v>515393</v>
       </c>
       <c r="H4" s="1">
         <v>1</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
       <c r="J4" s="1">
         <v>8</v>
@@ -3018,31 +2958,31 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>515384</v>
+        <v>515394</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>199</v>
+        <v>176</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>200</v>
+        <v>177</v>
       </c>
       <c r="E5" s="1">
-        <v>515384</v>
+        <v>515394</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>202</v>
+        <v>179</v>
       </c>
       <c r="G5" s="1">
-        <v>515384</v>
+        <v>515394</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="J5" s="1">
         <v>9</v>

</xml_diff>